<commit_message>
fixing the enum issues
</commit_message>
<xml_diff>
--- a/crowd_certain/outputs/final_figures/figure_metrics_mean_over_seeds_per_dataset_per_worker_ACC/figure_metrics_mean_over_seeds_per_dataset_per_worker_ACC.xlsx
+++ b/crowd_certain/outputs/final_figures/figure_metrics_mean_over_seeds_per_dataset_per_worker_ACC/figure_metrics_mean_over_seeds_per_dataset_per_worker_ACC.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,10 +452,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8930620761606677</v>
+        <v>0.9123630672926448</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9823589743589743</v>
+        <v>0.9769230769230769</v>
       </c>
     </row>
     <row r="3">
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7219613980177361</v>
+        <v>0.6525821596244131</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7292307692307692</v>
+        <v>0.6621538461538461</v>
       </c>
     </row>
     <row r="4">
@@ -478,10 +478,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.7219613980177361</v>
+        <v>0.6525821596244131</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7292307692307692</v>
+        <v>0.6621538461538461</v>
       </c>
     </row>
     <row r="5">
@@ -491,10 +491,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.782472613458529</v>
+        <v>0.7535211267605634</v>
       </c>
       <c r="C5" t="n">
-        <v>0.762051282051282</v>
+        <v>0.7489230769230769</v>
       </c>
     </row>
     <row r="6">
@@ -504,10 +504,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.7219613980177361</v>
+        <v>0.6525821596244131</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7292307692307692</v>
+        <v>0.6621538461538461</v>
       </c>
     </row>
     <row r="7">
@@ -517,10 +517,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8085550339071466</v>
+        <v>0.7574334898278561</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7965128205128206</v>
+        <v>0.7267692307692308</v>
       </c>
     </row>
     <row r="8">
@@ -530,62 +530,49 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.7219613980177361</v>
+        <v>0.6525821596244131</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7292307692307692</v>
+        <v>0.6621538461538461</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>GLAD</t>
+          <t>ZeroBasedSkill</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.7219613980177361</v>
+        <v>0.6525821596244131</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7292307692307692</v>
+        <v>0.6621538461538461</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>ZeroBasedSkill</t>
+          <t>MajorityVote</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.7219613980177361</v>
+        <v>0.6525821596244131</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7292307692307692</v>
+        <v>0.6621538461538461</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>MajorityVote</t>
+          <t>DawidSkene</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.7219613980177361</v>
+        <v>0.7660406885758999</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7292307692307692</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>DawidSkene</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0.8038601982263954</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.7669743589743589</v>
+        <v>0.7489230769230769</v>
       </c>
     </row>
   </sheetData>

</xml_diff>